<commit_message>
upgrade to POI 3.10
</commit_message>
<xml_diff>
--- a/spec/data/various_samples.xlsx
+++ b/spec/data/various_samples.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="720" windowWidth="21080" windowHeight="9780" activeTab="2"/>
+    <workbookView xWindow="25520" yWindow="-3100" windowWidth="38400" windowHeight="21160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="text &amp; pic" sheetId="1" r:id="rId1"/>
@@ -12,15 +12,16 @@
     <sheet name="dates" sheetId="3" r:id="rId3"/>
     <sheet name="bools &amp; errors" sheetId="4" r:id="rId4"/>
     <sheet name="high refs" sheetId="5" r:id="rId5"/>
+    <sheet name="newfeatures" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="four_times_six">'high refs'!$AO$624</definedName>
     <definedName name="NAMES">'bools &amp; errors'!$D$2:$D$11</definedName>
     <definedName name="nums">'high refs'!$AP$619:$AP$631</definedName>
   </definedNames>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>This</t>
   </si>
@@ -86,23 +87,39 @@
   <si>
     <t>This is some text</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>ONE</t>
+  </si>
+  <si>
+    <t>TWO</t>
+  </si>
+  <si>
+    <t>THREE</t>
+  </si>
+  <si>
+    <t>FOUR</t>
+  </si>
+  <si>
+    <t>LOOKUP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="mmmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="171" formatCode="m/d"/>
-    <numFmt numFmtId="172" formatCode="dd\-mmm\-yy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="m/d"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,16 +169,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -494,14 +511,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -544,7 +561,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -552,14 +569,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
@@ -834,11 +851,10 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -846,14 +862,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.83203125" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
@@ -1084,11 +1100,10 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -1096,14 +1111,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="21.6640625" customWidth="1"/>
   </cols>
@@ -1191,12 +1206,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -1204,14 +1218,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="AM619:AP631"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="AE612" workbookViewId="0">
       <selection activeCell="AO624" sqref="AO624"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="619" spans="39:42">
       <c r="AM619" t="s">
@@ -1334,14 +1348,98 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F6" si="0">IFERROR(VLOOKUP(A2,$A$1:$B$5,2,FALSE),"NOT FOUND")</f>
+        <v>ONE</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>TWO</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>THREE</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>FOUR</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>NOT FOUND</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>